<commit_message>
Completa calculos oligoelementos y vitaminas
Pone en funcionamiento los mismo, Además corregimos los macronutrientes para dietas de 500 gr peso bruto
</commit_message>
<xml_diff>
--- a/Guia_versiones.xlsx
+++ b/Guia_versiones.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>FECHA</t>
   </si>
@@ -46,6 +46,12 @@
   </si>
   <si>
     <t>Elimina necesidad de tabla Menu, incrementa campos en tabla Clasificacion_animal, y desarrolla consulta de menu</t>
+  </si>
+  <si>
+    <t>0616YjosetorresMAN11</t>
+  </si>
+  <si>
+    <t>Completa los calculos de vitamina y corrige % de macronutrientes en dieta de 500 gr</t>
   </si>
 </sst>
 </file>
@@ -364,10 +370,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -420,6 +426,17 @@
         <v>8</v>
       </c>
     </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>44729</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
finaliza access y inicia proy php
</commit_message>
<xml_diff>
--- a/Guia_versiones.xlsx
+++ b/Guia_versiones.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>FECHA</t>
   </si>
@@ -52,6 +52,12 @@
   </si>
   <si>
     <t>Completa los calculos de vitamina y corrige % de macronutrientes en dieta de 500 gr</t>
+  </si>
+  <si>
+    <t>Tarea_I_BIM_II_Ingenieria_Software</t>
+  </si>
+  <si>
+    <t>Presentación de proyecto inicial</t>
   </si>
 </sst>
 </file>
@@ -370,10 +376,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -395,45 +401,56 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>44726</v>
+        <v>44723</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>44727</v>
+        <v>44726</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>44728</v>
+        <v>44727</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
+        <v>44728</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
         <v>44729</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
         <v>9</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C6" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>